<commit_message>
Fixed error for a kicker's team value
</commit_message>
<xml_diff>
--- a/data/csv/cfb_team.xlsx
+++ b/data/csv/cfb_team.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\data_projects\cfb-analysis\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\data_projects\cfb-analysis\data\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BEB4D7-3FD4-44F0-9DC9-B4CDAFF0A53B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD92A627-8A84-469A-BFA5-0BCB4C13E2FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{9902822A-833C-4F31-A1F2-E8A6A5C2541E}"/>
   </bookViews>
@@ -1087,7 +1087,7 @@
   <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3779,10 +3779,10 @@
         <v>196</v>
       </c>
       <c r="G84" t="s">
+        <v>196</v>
+      </c>
+      <c r="H84" t="s">
         <v>197</v>
-      </c>
-      <c r="H84" t="s">
-        <v>104</v>
       </c>
       <c r="I84" t="s">
         <v>230</v>
@@ -3811,7 +3811,7 @@
         <v>196</v>
       </c>
       <c r="G85" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H85" t="s">
         <v>197</v>
@@ -3843,7 +3843,7 @@
         <v>196</v>
       </c>
       <c r="G86" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H86" t="s">
         <v>197</v>

</xml_diff>